<commit_message>
Pop up bar width
</commit_message>
<xml_diff>
--- a/Design/Testing/Game Page Test.xlsx
+++ b/Design/Testing/Game Page Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhodr\Desktop\MMP\Design\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328D535F-A8D4-4903-9EC5-42AD6BBDC6EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5F4F83-FCA9-4D1F-BA0E-C322A971C01F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="93">
   <si>
     <t>Test Number</t>
   </si>
@@ -298,6 +298,12 @@
   </si>
   <si>
     <t>If two squares have the answer in them, the user could click the wrong square and not gain a point for it</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Unknown, the tab somtimes completely crashes and nothing was able to detect the reason for the crash</t>
   </si>
 </sst>
 </file>
@@ -707,20 +713,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="37" style="1" customWidth="1"/>
-    <col min="3" max="4" width="41.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="39.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="40" style="1" customWidth="1"/>
-    <col min="7" max="7" width="35.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="32.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.5703125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="15.28515625" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -844,7 +850,7 @@
       </c>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -867,10 +873,10 @@
         <v>32</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>6</v>
+        <v>91</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>7</v>
+        <v>92</v>
       </c>
       <c r="J5" s="3"/>
     </row>

</xml_diff>